<commit_message>
Update inference, menambahkan figure
</commit_message>
<xml_diff>
--- a/Result_Kombinasi_Model.xlsx
+++ b/Result_Kombinasi_Model.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,40 +436,35 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>praklasifikasi</t>
+          <t>models</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>klasifikasi</t>
+          <t>accuracy</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>accuracy</t>
+          <t>recall</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>recall</t>
+          <t>precision</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>precision</t>
+          <t>f1_score</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>f1_score</t>
+          <t>average_runtime</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>average_runtime</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>median_runtime</t>
         </is>
@@ -478,181 +473,151 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>mamdani</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>mlp</t>
-        </is>
+          <t>['mamdani', 'mlp']</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.806577480490524</v>
       </c>
       <c r="C2" t="n">
         <v>0.806577480490524</v>
       </c>
       <c r="D2" t="n">
-        <v>0.813185301117604</v>
+        <v>0.8125072957494913</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8098460247140107</v>
+        <v>0.8069127034461214</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8089371816369816</v>
+        <v>0.2663744926452637</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5638533532619476</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.2692739963531494</v>
+        <v>0.1319910287857056</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>mamdani</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>lgbm</t>
-        </is>
+          <t>['mamdani', 'lgbm']</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.8344481605351171</v>
       </c>
       <c r="C3" t="n">
         <v>0.8344481605351171</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8379428609879755</v>
+        <v>0.8361176842296993</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8317233073158437</v>
+        <v>0.8340194950146642</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8334715670587792</v>
+        <v>0.3190764278173447</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6374644011259079</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.2833765745162964</v>
+        <v>0.1499724388122559</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>lr</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>mlp</t>
-        </is>
+          <t>['lr', 'mlp']</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.7987736900780379</v>
       </c>
       <c r="C4" t="n">
         <v>0.7987736900780379</v>
       </c>
       <c r="D4" t="n">
-        <v>0.800312628638861</v>
+        <v>0.8020056261781602</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8017073994914107</v>
+        <v>0.798970837990839</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7997230696183516</v>
+        <v>0.2872806489467621</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5516850739717484</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.2619267702102661</v>
+        <v>0.1328588724136353</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>lr</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>lgbm</t>
-        </is>
+          <t>['lr', 'lgbm']</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.8255295429208472</v>
       </c>
       <c r="C5" t="n">
         <v>0.8255295429208472</v>
       </c>
       <c r="D5" t="n">
-        <v>0.824047693621707</v>
+        <v>0.8261889021608652</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8240754659218852</v>
+        <v>0.8253038499871026</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8235537970161545</v>
+        <v>0.345859083533287</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6104085654020309</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.2650258541107178</v>
+        <v>0.1665419340133667</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>dt</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>mlp</t>
-        </is>
+          <t>['dt', 'mlp']</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.8132664437012264</v>
       </c>
       <c r="C6" t="n">
         <v>0.8132664437012264</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8296766292346239</v>
+        <v>0.8318556751371609</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8218600671987574</v>
+        <v>0.8127850574242346</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8151554745522535</v>
+        <v>0.2706254035234451</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5225788027048111</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.239149808883667</v>
+        <v>0.1317030191421509</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>dt</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>lgbm</t>
-        </is>
+          <t>['dt', 'lgbm']</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.8355629877369007</v>
       </c>
       <c r="C7" t="n">
         <v>0.8355629877369007</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8495056717685716</v>
+        <v>0.849953478282931</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8386154899527423</v>
+        <v>0.8348438778681438</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8350840353448495</v>
+        <v>0.3602471113204956</v>
       </c>
       <c r="G7" t="n">
-        <v>0.5889845281839371</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.2851012945175171</v>
+        <v>0.1784284114837646</v>
       </c>
     </row>
     <row r="8">
@@ -661,58 +626,48 @@
           <t>lgbm</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>mlp</t>
-        </is>
+      <c r="B8" t="n">
+        <v>0.9035674470457079</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8210702341137124</v>
+        <v>0.9035674470457079</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8248666480450444</v>
+        <v>0.90657404350533</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8242076560769274</v>
+        <v>0.9037620202233</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8221936551342065</v>
+        <v>0.4533237308263779</v>
       </c>
       <c r="G8" t="n">
-        <v>0.6441795855760575</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.2787847518920898</v>
+        <v>0.1842628717422485</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>lgbm</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>lgbm</t>
-        </is>
+          <t>mlp</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.875139353400223</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8389074693422519</v>
+        <v>0.875139353400223</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8406057110288897</v>
+        <v>0.89047978087285</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8375829032393414</v>
+        <v>0.876280832967023</v>
       </c>
       <c r="F9" t="n">
-        <v>0.8389197006815888</v>
+        <v>0.3528055310249328</v>
       </c>
       <c r="G9" t="n">
-        <v>0.6420337796211243</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.2727527618408203</v>
+        <v>0.1454615592956543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>